<commit_message>
list of customers that need to be alerted for no supply
</commit_message>
<xml_diff>
--- a/maven_ski_shop_data.xlsx
+++ b/maven_ski_shop_data.xlsx
@@ -1,23 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisb/Documents/Maven/Python_Foundations_Materials/Course_Assignments/Section12_Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511A8B10-81B8-5548-BE4A-4FB9A60555C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{511A8B10-81B8-5548-BE4A-4FB9A60555C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24C04FD7-AA29-4A40-8D37-85C56FB4F39C}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1100" windowWidth="38400" windowHeight="19560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-1100" windowWidth="38400" windowHeight="19560" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item_Info" sheetId="1" r:id="rId1"/>
     <sheet name="Inventory_Levels" sheetId="2" r:id="rId2"/>
     <sheet name="Orders_Info" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -241,7 +257,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,11 +294,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,13 +608,13 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -637,7 +654,7 @@
         <v>5.27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>10002</v>
       </c>
@@ -657,7 +674,7 @@
         <v>8.7899999999999991</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>10003</v>
       </c>
@@ -677,7 +694,7 @@
         <v>17.59</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>10004</v>
       </c>
@@ -697,7 +714,7 @@
         <v>21.99</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>10005</v>
       </c>
@@ -717,7 +734,7 @@
         <v>87.99</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>10006</v>
       </c>
@@ -737,7 +754,7 @@
         <v>70.39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>10007</v>
       </c>
@@ -757,7 +774,7 @@
         <v>105.59</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>10008</v>
       </c>
@@ -777,7 +794,7 @@
         <v>87.99</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>10009</v>
       </c>
@@ -797,7 +814,7 @@
         <v>175.99</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10010</v>
       </c>
@@ -817,7 +834,7 @@
         <v>527.99</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>10011</v>
       </c>
@@ -837,7 +854,7 @@
         <v>114.39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>10012</v>
       </c>
@@ -857,7 +874,7 @@
         <v>131.99</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>10013</v>
       </c>
@@ -890,14 +907,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -905,7 +922,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -913,7 +930,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>10002</v>
       </c>
@@ -921,7 +938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>10003</v>
       </c>
@@ -929,7 +946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>10004</v>
       </c>
@@ -937,7 +954,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>10005</v>
       </c>
@@ -945,7 +962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>10006</v>
       </c>
@@ -953,7 +970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>10007</v>
       </c>
@@ -961,7 +978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>10008</v>
       </c>
@@ -969,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>10009</v>
       </c>
@@ -977,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>10010</v>
       </c>
@@ -985,7 +1002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>10011</v>
       </c>
@@ -993,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>10012</v>
       </c>
@@ -1011,15 +1028,15 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="H2" sqref="H2:H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1045,7 +1062,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>100000</v>
       </c>
@@ -1061,11 +1078,11 @@
       <c r="G2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>100001</v>
       </c>
@@ -1081,11 +1098,11 @@
       <c r="G3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>100002</v>
       </c>
@@ -1101,11 +1118,11 @@
       <c r="G4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>100003</v>
       </c>
@@ -1121,11 +1138,11 @@
       <c r="G5" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>100004</v>
       </c>
@@ -1141,12 +1158,12 @@
       <c r="G6" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <v>10001</v>
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>100005</v>
       </c>
@@ -1162,11 +1179,11 @@
       <c r="G7" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
         <v>10010</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>100006</v>
       </c>
@@ -1182,11 +1199,11 @@
       <c r="G8" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <v>10004</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>100007</v>
       </c>
@@ -1202,12 +1219,12 @@
       <c r="G9" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="4" t="s">
         <v>51</v>
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>100008</v>
       </c>
@@ -1223,11 +1240,11 @@
       <c r="G10" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <v>10005</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>100009</v>
       </c>
@@ -1243,11 +1260,11 @@
       <c r="G11" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>100010</v>
       </c>
@@ -1263,11 +1280,11 @@
       <c r="G12" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>100011</v>
       </c>
@@ -1283,11 +1300,11 @@
       <c r="G13" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>10005</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>100012</v>
       </c>
@@ -1303,11 +1320,11 @@
       <c r="G14" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>100013</v>
       </c>
@@ -1323,11 +1340,11 @@
       <c r="G15" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>100014</v>
       </c>
@@ -1343,11 +1360,11 @@
       <c r="G16" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="4">
         <v>10014</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>100020</v>
       </c>
@@ -1363,11 +1380,11 @@
       <c r="G17" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
         <v>10007</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>100021</v>
       </c>
@@ -1383,11 +1400,11 @@
       <c r="G18" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="4">
         <v>10010</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>100022</v>
       </c>
@@ -1403,11 +1420,11 @@
       <c r="G19" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>100023</v>
       </c>
@@ -1423,11 +1440,11 @@
       <c r="G20" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="4">
         <v>10004</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>100024</v>
       </c>
@@ -1443,11 +1460,11 @@
       <c r="G21" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>10005</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>100025</v>
       </c>
@@ -1463,11 +1480,11 @@
       <c r="G22" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="4">
         <v>10008</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>100026</v>
       </c>
@@ -1483,11 +1500,11 @@
       <c r="G23" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="4">
         <v>10001</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>100027</v>
       </c>
@@ -1503,11 +1520,11 @@
       <c r="G24" t="s">
         <v>43</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="4">
         <v>10002</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>100031</v>
       </c>
@@ -1523,11 +1540,11 @@
       <c r="G25" t="s">
         <v>40</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>100032</v>
       </c>
@@ -1543,11 +1560,11 @@
       <c r="G26" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="4">
         <v>10006</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>100033</v>
       </c>
@@ -1563,11 +1580,11 @@
       <c r="G27" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>100034</v>
       </c>
@@ -1583,7 +1600,7 @@
       <c r="G28" t="s">
         <v>40</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="4">
         <v>10014</v>
       </c>
     </row>

</xml_diff>